<commit_message>
references #4 Revise data model.
</commit_message>
<xml_diff>
--- a/doc/drop_all_tables.xlsx
+++ b/doc/drop_all_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjg994/Documents/source/redcap2omop/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50405335-966F-D349-BC86-5032E3E21337}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A512F4EB-16BE-AC4A-9A7A-D7122BBE9753}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{FD8A4D80-FF6B-7046-BDFE-BE595F8073DA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>ar_internal_metadata</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>redcap_source_links</t>
+  </si>
+  <si>
+    <t>redcap_records_tmp_1</t>
   </si>
 </sst>
 </file>
@@ -540,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A31C0B-F15F-A245-8B8C-E2CB9577C12E}">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B55" sqref="B1:B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -552,128 +555,128 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B1" t="str">
         <f>CONCATENATE("DROP TABLE ",A1, " CASCADE;")</f>
-        <v>DROP TABLE schema_migrations CASCADE;</v>
+        <v>DROP TABLE domain CASCADE;</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B59" si="0">CONCATENATE("DROP TABLE ",A2, " CASCADE;")</f>
-        <v>DROP TABLE ar_internal_metadata CASCADE;</v>
+        <v>DROP TABLE vocabulary CASCADE;</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_projects CASCADE;</v>
+        <v>DROP TABLE redcap_records_tmp_1 CASCADE;</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_data_dictionaries CASCADE;</v>
+        <v>DROP TABLE care_site CASCADE;</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_variable_choices CASCADE;</v>
+        <v>DROP TABLE device_exposure CASCADE;</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_variables CASCADE;</v>
+        <v>DROP TABLE schema_migrations CASCADE;</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE concept CASCADE;</v>
+        <v>DROP TABLE ar_internal_metadata CASCADE;</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE vocabulary CASCADE;</v>
+        <v>DROP TABLE redcap_data_dictionaries CASCADE;</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE domain CASCADE;</v>
+        <v>DROP TABLE concept CASCADE;</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE concept_class CASCADE;</v>
+        <v>DROP TABLE concept_relationship CASCADE;</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE concept_relationship CASCADE;</v>
+        <v>DROP TABLE concept_ancestor CASCADE;</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE relationship CASCADE;</v>
+        <v>DROP TABLE drug_strength CASCADE;</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE concept_synonym CASCADE;</v>
+        <v>DROP TABLE drug_era CASCADE;</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE concept_ancestor CASCADE;</v>
+        <v>DROP TABLE dose_era CASCADE;</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -687,359 +690,362 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE drug_strength CASCADE;</v>
+        <v>DROP TABLE metadata CASCADE;</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE cohort_definition CASCADE;</v>
+        <v>DROP TABLE cdm_source CASCADE;</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE attribute_definition CASCADE;</v>
+        <v>DROP TABLE cohort_definition CASCADE;</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE cdm_source CASCADE;</v>
+        <v>DROP TABLE person CASCADE;</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE metadata CASCADE;</v>
+        <v>DROP TABLE visit_detail CASCADE;</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE person CASCADE;</v>
+        <v>DROP TABLE procedure_occurrence CASCADE;</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE observation_period CASCADE;</v>
+        <v>DROP TABLE fact_relationship CASCADE;</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE specimen CASCADE;</v>
+        <v>DROP TABLE location CASCADE;</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE death CASCADE;</v>
+        <v>DROP TABLE provider CASCADE;</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE visit_occurrence CASCADE;</v>
+        <v>DROP TABLE concept_class CASCADE;</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE visit_detail CASCADE;</v>
+        <v>DROP TABLE relationship CASCADE;</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE procedure_occurrence CASCADE;</v>
+        <v>DROP TABLE cohort CASCADE;</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE drug_exposure CASCADE;</v>
+        <v>DROP TABLE cohort_attribute CASCADE;</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE device_exposure CASCADE;</v>
+        <v>DROP TABLE cost CASCADE;</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE condition_occurrence CASCADE;</v>
+        <v>DROP TABLE concept_synonym CASCADE;</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE measurement CASCADE;</v>
+        <v>DROP TABLE attribute_definition CASCADE;</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE note CASCADE;</v>
+        <v>DROP TABLE observation_period CASCADE;</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE note_nlp CASCADE;</v>
+        <v>DROP TABLE death CASCADE;</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE fact_relationship CASCADE;</v>
+        <v>DROP TABLE specimen CASCADE;</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE location CASCADE;</v>
+        <v>DROP TABLE visit_occurrence CASCADE;</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE care_site CASCADE;</v>
+        <v>DROP TABLE redcap_variables CASCADE;</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE provider CASCADE;</v>
+        <v>DROP TABLE redcap_variable_choices CASCADE;</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE payer_plan_period CASCADE;</v>
+        <v>DROP TABLE omop_tables CASCADE;</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE cost CASCADE;</v>
+        <v>DROP TABLE omop_columns CASCADE;</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE cohort CASCADE;</v>
+        <v>DROP TABLE redcap_variable_maps CASCADE;</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE cohort_attribute CASCADE;</v>
+        <v>DROP TABLE redcap_variable_choice_maps CASCADE;</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE drug_era CASCADE;</v>
+        <v>DROP TABLE redcap_variable_child_maps CASCADE;</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE dose_era CASCADE;</v>
+        <v>DROP TABLE redcap_events CASCADE;</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE condition_era CASCADE;</v>
+        <v>DROP TABLE redcap_event_maps CASCADE;</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE observation CASCADE;</v>
+        <v>DROP TABLE redcap_event_map_dependents CASCADE;</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE omop_tables CASCADE;</v>
+        <v>DROP TABLE redcap_source_links CASCADE;</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE omop_columns CASCADE;</v>
+        <v>DROP TABLE redcap_projects CASCADE;</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_variable_maps CASCADE;</v>
+        <v>DROP TABLE drug_exposure CASCADE;</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_variable_choice_maps CASCADE;</v>
+        <v>DROP TABLE condition_occurrence CASCADE;</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_variable_child_maps CASCADE;</v>
+        <v>DROP TABLE measurement CASCADE;</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_events CASCADE;</v>
+        <v>DROP TABLE note CASCADE;</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_event_maps CASCADE;</v>
+        <v>DROP TABLE payer_plan_period CASCADE;</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_event_map_dependents CASCADE;</v>
+        <v>DROP TABLE observation CASCADE;</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_source_links CASCADE;</v>
+        <v>DROP TABLE note_nlp CASCADE;</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE  CASCADE;</v>
+        <v>DROP TABLE condition_era CASCADE;</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
references #33 Finish first draft of CCC19 mappings.
</commit_message>
<xml_diff>
--- a/doc/drop_all_tables.xlsx
+++ b/doc/drop_all_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjg994/Documents/source/redcap2omop/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A512F4EB-16BE-AC4A-9A7A-D7122BBE9753}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E10ED6-8DDE-1B41-9B43-0944DD7EF800}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{FD8A4D80-FF6B-7046-BDFE-BE595F8073DA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>ar_internal_metadata</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>redcap_records_tmp_1</t>
+  </si>
+  <si>
+    <t>redcap_derived_dates</t>
+  </si>
+  <si>
+    <t>redcap_derived_date_choice_offset_mappings</t>
+  </si>
+  <si>
+    <t>redcap_records_tmp_5</t>
   </si>
 </sst>
 </file>
@@ -543,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A31C0B-F15F-A245-8B8C-E2CB9577C12E}">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B55" sqref="B1:B55"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B58" sqref="B1:B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,11 +564,11 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B1" t="str">
         <f>CONCATENATE("DROP TABLE ",A1, " CASCADE;")</f>
-        <v>DROP TABLE domain CASCADE;</v>
+        <v>DROP TABLE concept CASCADE;</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -573,164 +582,164 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_records_tmp_1 CASCADE;</v>
+        <v>DROP TABLE domain CASCADE;</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE care_site CASCADE;</v>
+        <v>DROP TABLE concept_class CASCADE;</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE device_exposure CASCADE;</v>
+        <v>DROP TABLE relationship CASCADE;</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE schema_migrations CASCADE;</v>
+        <v>DROP TABLE drug_era CASCADE;</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE ar_internal_metadata CASCADE;</v>
+        <v>DROP TABLE concept_synonym CASCADE;</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_data_dictionaries CASCADE;</v>
+        <v>DROP TABLE redcap_records_tmp_1 CASCADE;</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE concept CASCADE;</v>
+        <v>DROP TABLE concept_ancestor CASCADE;</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE concept_relationship CASCADE;</v>
+        <v>DROP TABLE drug_strength CASCADE;</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE concept_ancestor CASCADE;</v>
+        <v>DROP TABLE schema_migrations CASCADE;</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE drug_strength CASCADE;</v>
+        <v>DROP TABLE ar_internal_metadata CASCADE;</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE drug_era CASCADE;</v>
+        <v>DROP TABLE concept_relationship CASCADE;</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE dose_era CASCADE;</v>
+        <v>DROP TABLE metadata CASCADE;</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE source_to_concept_map CASCADE;</v>
+        <v>DROP TABLE cdm_source CASCADE;</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE metadata CASCADE;</v>
+        <v>DROP TABLE visit_detail CASCADE;</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE cdm_source CASCADE;</v>
+        <v>DROP TABLE cohort_definition CASCADE;</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE cohort_definition CASCADE;</v>
+        <v>DROP TABLE death CASCADE;</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE person CASCADE;</v>
+        <v>DROP TABLE observation_period CASCADE;</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE visit_detail CASCADE;</v>
+        <v>DROP TABLE person CASCADE;</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -744,326 +753,335 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE fact_relationship CASCADE;</v>
+        <v>DROP TABLE source_to_concept_map CASCADE;</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE location CASCADE;</v>
+        <v>DROP TABLE specimen CASCADE;</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE provider CASCADE;</v>
+        <v>DROP TABLE visit_occurrence CASCADE;</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE concept_class CASCADE;</v>
+        <v>DROP TABLE care_site CASCADE;</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE relationship CASCADE;</v>
+        <v>DROP TABLE cohort CASCADE;</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE cohort CASCADE;</v>
+        <v>DROP TABLE cohort_attribute CASCADE;</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE cohort_attribute CASCADE;</v>
+        <v>DROP TABLE condition_era CASCADE;</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE cost CASCADE;</v>
+        <v>DROP TABLE condition_occurrence CASCADE;</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE concept_synonym CASCADE;</v>
+        <v>DROP TABLE cost CASCADE;</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE attribute_definition CASCADE;</v>
+        <v>DROP TABLE device_exposure CASCADE;</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE observation_period CASCADE;</v>
+        <v>DROP TABLE dose_era CASCADE;</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE death CASCADE;</v>
+        <v>DROP TABLE drug_exposure CASCADE;</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE specimen CASCADE;</v>
+        <v>DROP TABLE fact_relationship CASCADE;</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE visit_occurrence CASCADE;</v>
+        <v>DROP TABLE location CASCADE;</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_variables CASCADE;</v>
+        <v>DROP TABLE measurement CASCADE;</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_variable_choices CASCADE;</v>
+        <v>DROP TABLE note CASCADE;</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE omop_tables CASCADE;</v>
+        <v>DROP TABLE note_nlp CASCADE;</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE omop_columns CASCADE;</v>
+        <v>DROP TABLE observation CASCADE;</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_variable_maps CASCADE;</v>
+        <v>DROP TABLE payer_plan_period CASCADE;</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_variable_choice_maps CASCADE;</v>
+        <v>DROP TABLE provider CASCADE;</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_variable_child_maps CASCADE;</v>
+        <v>DROP TABLE redcap_projects CASCADE;</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_events CASCADE;</v>
+        <v>DROP TABLE redcap_data_dictionaries CASCADE;</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_event_maps CASCADE;</v>
+        <v>DROP TABLE redcap_variable_choice_maps CASCADE;</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_event_map_dependents CASCADE;</v>
+        <v>DROP TABLE redcap_variable_choices CASCADE;</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_source_links CASCADE;</v>
+        <v>DROP TABLE omop_tables CASCADE;</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE redcap_projects CASCADE;</v>
+        <v>DROP TABLE omop_columns CASCADE;</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE drug_exposure CASCADE;</v>
+        <v>DROP TABLE redcap_variable_child_maps CASCADE;</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE condition_occurrence CASCADE;</v>
+        <v>DROP TABLE redcap_events CASCADE;</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE measurement CASCADE;</v>
+        <v>DROP TABLE redcap_variables CASCADE;</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE note CASCADE;</v>
+        <v>DROP TABLE attribute_definition CASCADE;</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE payer_plan_period CASCADE;</v>
+        <v>DROP TABLE redcap_event_maps CASCADE;</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE observation CASCADE;</v>
+        <v>DROP TABLE redcap_event_map_dependents CASCADE;</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE note_nlp CASCADE;</v>
+        <v>DROP TABLE redcap_source_links CASCADE;</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE condition_era CASCADE;</v>
+        <v>DROP TABLE redcap_variable_maps CASCADE;</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
       <c r="B56" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE  CASCADE;</v>
+        <v>DROP TABLE redcap_derived_dates CASCADE;</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
       <c r="B57" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE  CASCADE;</v>
+        <v>DROP TABLE redcap_derived_date_choice_offset_mappings CASCADE;</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
       <c r="B58" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE  CASCADE;</v>
+        <v>DROP TABLE redcap_records_tmp_5 CASCADE;</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>